<commit_message>
Chapters completed. Minor revisions.
</commit_message>
<xml_diff>
--- a/March 3, 2022/Expences Documentation/Expences.xlsx
+++ b/March 3, 2022/Expences Documentation/Expences.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Makoy files_DONT REMOVE\Computer-Engineering-Practice-and-Design-2\0_MARCH_3_2022\POF_Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Makoy files_DONT REMOVE\Computer-Engineering-Practice-and-Design-2\March 3, 2022\Expences Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A08E97-2EC0-4769-8E39-E0049780A108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A65A9F-E73C-45CF-B4D4-F80E206CFE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{34E937BC-3B4F-43D1-B580-D634078245D1}"/>
   </bookViews>
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89AC3C42-CD89-4EF1-9A03-CFA0B70CDF56}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,6 +549,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>200</v>
+      </c>
       <c r="B6">
         <v>200</v>
       </c>
@@ -563,6 +566,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>165</v>
+      </c>
       <c r="B7">
         <v>165</v>
       </c>
@@ -619,6 +625,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1000</v>
+      </c>
       <c r="B11">
         <v>1000</v>
       </c>
@@ -661,6 +670,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>40</v>
+      </c>
       <c r="B14">
         <v>40</v>
       </c>
@@ -717,6 +729,9 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>700</v>
+      </c>
       <c r="B18">
         <v>700</v>
       </c>

</xml_diff>